<commit_message>
Changed Burndown Spez and Test rep
</commit_message>
<xml_diff>
--- a/PLET_HoloM_ScrumTable.xlsx
+++ b/PLET_HoloM_ScrumTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocot\sciebo\CSN\PLET\Workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cocot\sciebo\CSN\PLET\Workshop\HoloM_repo\PLET20_HoloM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23EC81-ED89-4ED7-98C6-1E12A511D355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344CB3D-2933-468C-BD86-66BEBAFFAD31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="9030" windowWidth="19780" windowHeight="13420" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="4" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="285">
   <si>
     <t>Aufgabe</t>
   </si>
@@ -567,15 +567,6 @@
     <t>Mechanische Konstruktion des Mikroskops</t>
   </si>
   <si>
-    <t>Spez2</t>
-  </si>
-  <si>
-    <t>Spez3</t>
-  </si>
-  <si>
-    <t>Spez4</t>
-  </si>
-  <si>
     <t>Aufbau des Holo-Mikroskops</t>
   </si>
   <si>
@@ -781,30 +772,6 @@
   </si>
   <si>
     <t>Auswahl eines geeigneten Lasers</t>
-  </si>
-  <si>
-    <t>Spez12</t>
-  </si>
-  <si>
-    <t>Spez13</t>
-  </si>
-  <si>
-    <t>Spez14</t>
-  </si>
-  <si>
-    <t>Spez15</t>
-  </si>
-  <si>
-    <t>Spez16</t>
-  </si>
-  <si>
-    <t>Spez17</t>
-  </si>
-  <si>
-    <t>Spez18</t>
-  </si>
-  <si>
-    <t>Spez19</t>
   </si>
   <si>
     <t>Entspricht die Auflösung der Spezifikation (mind. 1080p)?</t>
@@ -865,12 +832,6 @@
 2) Auflistung aller benötigten Optik-Komponenten und deren Spezifikationen</t>
   </si>
   <si>
-    <t>Spez1 (siehe Product Backlog)</t>
-  </si>
-  <si>
-    <t>Test1 (siehe Product Backlog)</t>
-  </si>
-  <si>
     <t>Reichen die Recherche-Ergebnisse aus um ein generelles Verständnis über das Projekt zu erlangen?</t>
   </si>
   <si>
@@ -907,6 +868,129 @@
     <t xml:space="preserve">1) Rechenweg und eingehende Parameter offenlegen, um Nachvollziehbarkeit für den Prüfer zu gewährleisten
 2) Ebenfalls Berechnung der Maße offenlegen, zur Kontrolle durch Prüfer
 </t>
+  </si>
+  <si>
+    <t>Alle Spezifikationen und Testmethoden werden an dieser Stelle lediglich referenziert. Der Volltext findet sich bei den jeweiligen Arbeitspaketen im Product Backlog.</t>
+  </si>
+  <si>
+    <t>Spez AP 2</t>
+  </si>
+  <si>
+    <t>Spez AP 5</t>
+  </si>
+  <si>
+    <t>Spez AP 4</t>
+  </si>
+  <si>
+    <t>Spez AP 3</t>
+  </si>
+  <si>
+    <t>Spez AP 1</t>
+  </si>
+  <si>
+    <t>Spez AP 6</t>
+  </si>
+  <si>
+    <t>Spez AP 7</t>
+  </si>
+  <si>
+    <t>Spez AP 8</t>
+  </si>
+  <si>
+    <t>Spez AP 9</t>
+  </si>
+  <si>
+    <t>Spez AP 10</t>
+  </si>
+  <si>
+    <t>Spez AP 11</t>
+  </si>
+  <si>
+    <t>Spez AP 12</t>
+  </si>
+  <si>
+    <t>Spez AP 13</t>
+  </si>
+  <si>
+    <t>Spez AP 14</t>
+  </si>
+  <si>
+    <t>Spez AP 15</t>
+  </si>
+  <si>
+    <t>Spez AP 16</t>
+  </si>
+  <si>
+    <t>Spez AP 17</t>
+  </si>
+  <si>
+    <t>Spez AP 18</t>
+  </si>
+  <si>
+    <t>Spez AP 19</t>
+  </si>
+  <si>
+    <t>Spez AP 20</t>
+  </si>
+  <si>
+    <t>Test AP 1</t>
+  </si>
+  <si>
+    <t>Test AP 2</t>
+  </si>
+  <si>
+    <t>Test AP 3</t>
+  </si>
+  <si>
+    <t>Test AP 4</t>
+  </si>
+  <si>
+    <t>Test AP 5</t>
+  </si>
+  <si>
+    <t>Test AP 6</t>
+  </si>
+  <si>
+    <t>Test AP 7</t>
+  </si>
+  <si>
+    <t>Test AP 8</t>
+  </si>
+  <si>
+    <t>Test AP 9</t>
+  </si>
+  <si>
+    <t>Test AP 10</t>
+  </si>
+  <si>
+    <t>Test AP 11</t>
+  </si>
+  <si>
+    <t>Test AP 12</t>
+  </si>
+  <si>
+    <t>Test AP 13</t>
+  </si>
+  <si>
+    <t>Test AP 14</t>
+  </si>
+  <si>
+    <t>Test AP 15</t>
+  </si>
+  <si>
+    <t>Test AP 16</t>
+  </si>
+  <si>
+    <t>Test AP 17</t>
+  </si>
+  <si>
+    <t>Test AP 18</t>
+  </si>
+  <si>
+    <t>Test AP 19</t>
+  </si>
+  <si>
+    <t>Test AP 20</t>
   </si>
 </sst>
 </file>
@@ -1331,9 +1415,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1490,6 +1571,36 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1519,27 +1630,27 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1549,12 +1660,27 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1563,48 +1689,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -2031,13 +2115,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="77.5">
@@ -2048,13 +2132,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>159</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="62">
@@ -2065,13 +2149,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="62">
@@ -2082,13 +2166,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="93">
@@ -2099,13 +2183,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E6" s="72" t="s">
-        <v>236</v>
+        <v>223</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="46.5">
@@ -2119,10 +2203,10 @@
         <v>148</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="77.5">
@@ -2136,10 +2220,10 @@
         <v>147</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="93">
@@ -2153,10 +2237,10 @@
         <v>145</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="139.5">
@@ -2167,13 +2251,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="62">
@@ -2184,13 +2268,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="77.5">
@@ -2200,14 +2284,14 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="31" t="s">
         <v>146</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2284,7 +2368,7 @@
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
@@ -2324,7 +2408,7 @@
   </sheetPr>
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="200" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
@@ -2346,16 +2430,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="12" customFormat="1" ht="66" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
       <c r="I1" s="14"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -2386,13 +2470,13 @@
       <c r="H2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="I2" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="96"/>
     </row>
     <row r="3" spans="1:13" ht="139.5">
       <c r="A3" s="4">
@@ -2401,14 +2485,14 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="72" t="s">
-        <v>179</v>
+      <c r="C3" s="71" t="s">
+        <v>176</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F3" s="5">
         <v>3</v>
@@ -2424,14 +2508,14 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="72" t="s">
-        <v>180</v>
-      </c>
-      <c r="D4" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>241</v>
+      <c r="C4" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>230</v>
       </c>
       <c r="F4" s="5">
         <v>3</v>
@@ -2453,14 +2537,14 @@
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="72" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="72" t="s">
-        <v>239</v>
+      <c r="C5" s="71" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="71" t="s">
+        <v>228</v>
       </c>
       <c r="F5" s="4">
         <v>4</v>
@@ -2468,8 +2552,8 @@
       <c r="G5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="72" t="s">
-        <v>190</v>
+      <c r="H5" s="71" t="s">
+        <v>187</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>42</v>
@@ -2485,14 +2569,14 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="72" t="s">
-        <v>220</v>
-      </c>
-      <c r="D6" s="75" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>252</v>
+      <c r="C6" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>238</v>
+      </c>
+      <c r="E6" s="74" t="s">
+        <v>239</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
@@ -2500,8 +2584,8 @@
       <c r="G6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="72" t="s">
-        <v>191</v>
+      <c r="H6" s="71" t="s">
+        <v>188</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>44</v>
@@ -2517,14 +2601,14 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="72" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="75" t="s">
-        <v>253</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>254</v>
+      <c r="C7" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>240</v>
+      </c>
+      <c r="E7" s="74" t="s">
+        <v>241</v>
       </c>
       <c r="F7" s="4">
         <v>5</v>
@@ -2532,8 +2616,8 @@
       <c r="G7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="72" t="s">
-        <v>192</v>
+      <c r="H7" s="71" t="s">
+        <v>189</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>46</v>
@@ -2549,19 +2633,19 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="71" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="72" t="s">
-        <v>244</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>245</v>
+      <c r="E8" s="71" t="s">
+        <v>234</v>
       </c>
       <c r="F8" s="4">
         <v>3</v>
       </c>
-      <c r="H8" s="72"/>
+      <c r="H8" s="71"/>
       <c r="J8" s="4" t="s">
         <v>60</v>
       </c>
@@ -2576,14 +2660,14 @@
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="72" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="75" t="s">
-        <v>255</v>
-      </c>
-      <c r="E9" s="75" t="s">
-        <v>256</v>
+      <c r="C9" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>243</v>
       </c>
       <c r="F9" s="4">
         <v>4</v>
@@ -2591,8 +2675,8 @@
       <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="72" t="s">
-        <v>193</v>
+      <c r="H9" s="71" t="s">
+        <v>190</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>63</v>
@@ -2608,14 +2692,14 @@
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="72" t="s">
-        <v>250</v>
+      <c r="C10" s="71" t="s">
+        <v>237</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F10" s="4">
         <v>3</v>
@@ -2623,25 +2707,25 @@
       <c r="G10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="72" t="s">
-        <v>194</v>
+      <c r="H10" s="71" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="31">
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="72" t="s">
-        <v>196</v>
+      <c r="C11" s="71" t="s">
+        <v>193</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -2649,8 +2733,8 @@
       <c r="G11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="72" t="s">
-        <v>189</v>
+      <c r="H11" s="71" t="s">
+        <v>186</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>66</v>
@@ -2663,11 +2747,11 @@
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72" t="s">
-        <v>195</v>
+      <c r="C12" s="71" t="s">
+        <v>192</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>37</v>
@@ -2678,17 +2762,17 @@
       <c r="G12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="71" t="s">
         <v>141</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="84" t="s">
+      <c r="K12" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="88"/>
-      <c r="M12" s="89"/>
+      <c r="L12" s="97"/>
+      <c r="M12" s="98"/>
     </row>
     <row r="13" spans="1:13" ht="49.5" customHeight="1">
       <c r="A13" s="4">
@@ -2697,11 +2781,11 @@
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="72" t="s">
-        <v>152</v>
+      <c r="C13" s="71" t="s">
+        <v>149</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>37</v>
@@ -2712,15 +2796,15 @@
       <c r="G13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="72"/>
+      <c r="H13" s="71"/>
       <c r="I13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="84" t="s">
+      <c r="K13" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="90"/>
-      <c r="M13" s="91"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="100"/>
     </row>
     <row r="14" spans="1:13" ht="46.5">
       <c r="A14" s="4">
@@ -2729,11 +2813,11 @@
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="72" t="s">
-        <v>197</v>
+      <c r="C14" s="71" t="s">
+        <v>194</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>38</v>
@@ -2744,16 +2828,16 @@
       <c r="G14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="72"/>
-      <c r="I14" s="92" t="s">
+      <c r="H14" s="71"/>
+      <c r="I14" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="93"/>
-      <c r="K14" s="84" t="s">
+      <c r="J14" s="102"/>
+      <c r="K14" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="90"/>
-      <c r="M14" s="91"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="100"/>
     </row>
     <row r="15" spans="1:13" ht="46.5">
       <c r="A15" s="4">
@@ -2762,11 +2846,11 @@
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="72" t="s">
-        <v>199</v>
+      <c r="C15" s="71" t="s">
+        <v>196</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>38</v>
@@ -2777,7 +2861,7 @@
       <c r="G15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="72"/>
+      <c r="H15" s="71"/>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:13">
@@ -2787,14 +2871,14 @@
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>203</v>
       </c>
       <c r="F16" s="5">
         <v>5</v>
@@ -2802,7 +2886,7 @@
       <c r="G16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="72"/>
+      <c r="H16" s="71"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="4">
@@ -2811,14 +2895,14 @@
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -2826,7 +2910,7 @@
       <c r="G17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="72"/>
+      <c r="H17" s="71"/>
     </row>
     <row r="18" spans="1:8" ht="31">
       <c r="A18" s="4">
@@ -2835,14 +2919,14 @@
       <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="72" t="s">
-        <v>206</v>
+      <c r="C18" s="71" t="s">
+        <v>203</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F18" s="5">
         <v>3</v>
@@ -2850,7 +2934,7 @@
       <c r="G18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="72"/>
+      <c r="H18" s="71"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="4">
@@ -2859,14 +2943,14 @@
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="72" t="s">
-        <v>209</v>
+      <c r="C19" s="71" t="s">
+        <v>206</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F19" s="5">
         <v>6</v>
@@ -2874,7 +2958,7 @@
       <c r="G19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="72"/>
+      <c r="H19" s="71"/>
     </row>
     <row r="20" spans="1:8" ht="31">
       <c r="A20" s="4">
@@ -2883,14 +2967,14 @@
       <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="F20" s="5">
         <v>4</v>
@@ -2898,7 +2982,7 @@
       <c r="G20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="72"/>
+      <c r="H20" s="71"/>
     </row>
     <row r="21" spans="1:8" ht="31">
       <c r="A21" s="4">
@@ -2907,14 +2991,14 @@
       <c r="B21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>213</v>
+      <c r="C21" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>210</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F21" s="5">
         <v>7</v>
@@ -2922,7 +3006,7 @@
       <c r="G21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="72"/>
+      <c r="H21" s="71"/>
     </row>
     <row r="22" spans="1:8" ht="62">
       <c r="A22" s="4">
@@ -2931,14 +3015,14 @@
       <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="71" t="s">
         <v>146</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F22" s="5">
         <v>5</v>
@@ -2946,7 +3030,7 @@
       <c r="G22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="72"/>
+      <c r="H22" s="71"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="4">
@@ -2956,7 +3040,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3209,7 +3293,7 @@
       <c r="A64" s="4">
         <v>62</v>
       </c>
-      <c r="B64" s="32"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -3228,7 +3312,7 @@
       <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B66" s="32"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
@@ -3238,7 +3322,7 @@
       <c r="A67" s="4">
         <v>65</v>
       </c>
-      <c r="B67" s="32"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
@@ -3458,9 +3542,9 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -3481,11 +3565,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="97"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="7"/>
       <c r="E1" s="3" t="s">
         <v>35</v>
@@ -3553,12 +3637,12 @@
         <v>50</v>
       </c>
       <c r="M2" s="24"/>
-      <c r="N2" s="98" t="s">
+      <c r="N2" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
     </row>
     <row r="3" spans="1:17" ht="31">
       <c r="A3" s="7" t="s">
@@ -3605,10 +3689,10 @@
       <c r="M3" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
+      <c r="Q3" s="106"/>
     </row>
     <row r="4" spans="1:17" ht="68.5" customHeight="1">
       <c r="A4" s="4">
@@ -3617,28 +3701,28 @@
       <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="71" t="str">
         <f>IF(A4&gt;0,VLOOKUP(A4,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Wahl eines passenden Kameramoduls</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F4" s="4">
         <v>3</v>
       </c>
       <c r="M4" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="N4" s="99" t="s">
+        <v>265</v>
+      </c>
+      <c r="N4" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="108"/>
+      <c r="Q4" s="108"/>
     </row>
     <row r="5" spans="1:17" ht="63.5" customHeight="1">
       <c r="A5" s="4">
@@ -3647,20 +3731,22 @@
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="72" t="str">
+      <c r="C5" s="71" t="str">
         <f>IF(A5&gt;0,VLOOKUP(A5,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Auswahl eines passenden Mirkocontroller-Systems</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>149</v>
+      <c r="D5" s="82" t="s">
+        <v>245</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F5" s="4">
         <v>3</v>
       </c>
-      <c r="M5" s="26"/>
+      <c r="M5" s="25" t="s">
+        <v>266</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="9"/>
       <c r="P5" s="2"/>
@@ -3673,27 +3759,30 @@
       <c r="B6" s="21">
         <v>1</v>
       </c>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="71" t="str">
         <f>IF(A6&gt;0,VLOOKUP(A6,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Recherche: Prinzip von Holographie-Mikroskopen</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>182</v>
+        <v>250</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="M6" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="N6" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="94" t="s">
+      <c r="O6" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
+      <c r="P6" s="109"/>
+      <c r="Q6" s="109"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="4">
@@ -3702,15 +3791,18 @@
       <c r="B7" s="22">
         <v>2</v>
       </c>
-      <c r="C7" s="72" t="str">
+      <c r="C7" s="71" t="str">
         <f>IF(A7&gt;0,VLOOKUP(A7,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Auswahl eines geeigneten Lasers</v>
       </c>
-      <c r="D7" s="72" t="s">
-        <v>151</v>
+      <c r="D7" s="71" t="s">
+        <v>247</v>
       </c>
       <c r="F7" s="4">
         <v>3</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>268</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -3724,17 +3816,20 @@
       <c r="B8" s="22">
         <v>2</v>
       </c>
-      <c r="C8" s="72" t="str">
+      <c r="C8" s="71" t="str">
         <f>IF(A8&gt;0,VLOOKUP(A8,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Übertragung von Bilddaten auf Mirkokontroller</v>
       </c>
-      <c r="D8" s="72" t="s">
-        <v>150</v>
+      <c r="D8" s="71" t="s">
+        <v>248</v>
       </c>
       <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="N8" s="27" t="s">
+      <c r="M8" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="N8" s="26" t="s">
         <v>77</v>
       </c>
       <c r="O8" s="2"/>
@@ -3748,22 +3843,25 @@
       <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="72" t="str">
+      <c r="C9" s="71" t="str">
         <f>IF(A9&gt;0,VLOOKUP(A9,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Planung des Hardware Designs</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>182</v>
+        <v>246</v>
       </c>
       <c r="F9" s="4">
         <v>5</v>
       </c>
+      <c r="M9" s="25" t="s">
+        <v>269</v>
+      </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="94" t="s">
+      <c r="O9" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="4">
@@ -3772,15 +3870,18 @@
       <c r="B10" s="22">
         <v>2</v>
       </c>
-      <c r="C10" s="72" t="str">
+      <c r="C10" s="71" t="str">
         <f>IF(A10&gt;0,VLOOKUP(A10,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Planung/Berechnung des Optik Designs</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>183</v>
+        <v>251</v>
       </c>
       <c r="F10" s="4">
         <v>4</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>271</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -3794,15 +3895,18 @@
       <c r="B11" s="22">
         <v>2</v>
       </c>
-      <c r="C11" s="72" t="str">
+      <c r="C11" s="71" t="str">
         <f>IF(A11&gt;0,VLOOKUP(A11,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Konkrete Auswahl der benötigten Optik-Komponenten</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>184</v>
+        <v>252</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>272</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="9" t="s">
@@ -3818,15 +3922,18 @@
       <c r="B12" s="23">
         <v>3</v>
       </c>
-      <c r="C12" s="72" t="str">
+      <c r="C12" s="71" t="str">
         <f>IF(A12&gt;0,VLOOKUP(A12,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Testaufbau</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>185</v>
+        <v>253</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>273</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -3840,41 +3947,47 @@
       <c r="B13" s="23">
         <v>3</v>
       </c>
-      <c r="C13" s="72" t="str">
+      <c r="C13" s="71" t="str">
         <f>IF(A13&gt;0,VLOOKUP(A13,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Design der Konstruktion (Halterungen etc.)</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>186</v>
+        <v>254</v>
       </c>
       <c r="F13" s="4">
         <v>8</v>
       </c>
-      <c r="N13" s="27" t="s">
+      <c r="M13" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="N13" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="O13" s="94" t="s">
+      <c r="O13" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="76">
         <v>4</v>
       </c>
-      <c r="C14" s="72" t="str">
+      <c r="C14" s="71" t="str">
         <f>IF(A14&gt;0,VLOOKUP(A14,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Aufbau des Holo-Mikroskops</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>213</v>
+      <c r="D14" s="82" t="s">
+        <v>255</v>
       </c>
       <c r="F14" s="4">
         <v>3</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>275</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -3885,140 +3998,158 @@
       <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="77">
+      <c r="B15" s="76">
         <v>4</v>
       </c>
-      <c r="C15" s="72" t="str">
+      <c r="C15" s="71" t="str">
         <f>IF(A15&gt;0,VLOOKUP(A15,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Bereitstellung der Bilddaten an Leistungsstarken Prozessor</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>215</v>
+      <c r="D15" s="82" t="s">
+        <v>256</v>
       </c>
       <c r="F15" s="4">
         <v>6</v>
       </c>
-      <c r="N15" s="27" t="s">
+      <c r="M15" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="N15" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="O15" s="94" t="s">
+      <c r="O15" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="94"/>
+      <c r="P15" s="109"/>
+      <c r="Q15" s="109"/>
     </row>
     <row r="16" spans="1:17" ht="142.5" customHeight="1">
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="78">
+      <c r="B16" s="77">
         <v>5</v>
       </c>
-      <c r="C16" s="72" t="str">
+      <c r="C16" s="71" t="str">
         <f>IF(A16&gt;0,VLOOKUP(A16,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Entwicklung der Datenverarbeitung und Bildberechnung</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>221</v>
+      <c r="D16" s="82" t="s">
+        <v>257</v>
       </c>
       <c r="F16" s="4">
         <v>10</v>
       </c>
-      <c r="N16" s="27" t="s">
+      <c r="M16" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="N16" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="O16" s="94" t="s">
+      <c r="O16" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="P16" s="94"/>
-      <c r="Q16" s="94"/>
+      <c r="P16" s="109"/>
+      <c r="Q16" s="109"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="78">
+      <c r="B17" s="77">
         <v>5</v>
       </c>
-      <c r="C17" s="72" t="str">
+      <c r="C17" s="71" t="str">
         <f>IF(A17&gt;0,VLOOKUP(A17,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Design des Gehäuses</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>222</v>
+      <c r="D17" s="82" t="s">
+        <v>258</v>
       </c>
       <c r="F17" s="4">
         <v>5</v>
       </c>
-      <c r="N17" s="27"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="94"/>
+      <c r="M17" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="N17" s="26"/>
+      <c r="O17" s="109"/>
+      <c r="P17" s="109"/>
+      <c r="Q17" s="109"/>
     </row>
     <row r="18" spans="1:17" ht="54" customHeight="1">
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="79">
+      <c r="B18" s="78">
         <v>6</v>
       </c>
-      <c r="C18" s="72" t="str">
+      <c r="C18" s="71" t="str">
         <f>IF(A18&gt;0,VLOOKUP(A18,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Montage des Gehäuses</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>223</v>
+      <c r="D18" s="82" t="s">
+        <v>259</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
       </c>
-      <c r="N18" s="27" t="s">
+      <c r="M18" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="N18" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="94" t="s">
+      <c r="O18" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="P18" s="94"/>
-      <c r="Q18" s="94"/>
+      <c r="P18" s="109"/>
+      <c r="Q18" s="109"/>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="79">
+      <c r="B19" s="78">
         <v>6</v>
       </c>
-      <c r="C19" s="72" t="str">
+      <c r="C19" s="71" t="str">
         <f>IF(A19&gt;0,VLOOKUP(A19,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Konzeption automatisierte Justizierung</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>224</v>
+      <c r="D19" s="82" t="s">
+        <v>260</v>
       </c>
       <c r="F19" s="4">
         <v>3</v>
       </c>
-      <c r="N19" s="27"/>
-      <c r="O19" s="94"/>
-      <c r="P19" s="94"/>
-      <c r="Q19" s="94"/>
+      <c r="M19" s="25" t="s">
+        <v>280</v>
+      </c>
+      <c r="N19" s="26"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="109"/>
+      <c r="Q19" s="109"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="80">
+      <c r="B20" s="79">
         <v>7</v>
       </c>
-      <c r="C20" s="72" t="str">
+      <c r="C20" s="71" t="str">
         <f>IF(A20&gt;0,VLOOKUP(A20,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Umsetzung der Justizierung</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>225</v>
+      <c r="D20" s="82" t="s">
+        <v>261</v>
       </c>
       <c r="F20" s="4">
         <v>6</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>281</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -4029,18 +4160,21 @@
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="80">
+      <c r="B21" s="79">
         <v>7</v>
       </c>
-      <c r="C21" s="72" t="str">
+      <c r="C21" s="71" t="str">
         <f>IF(A21&gt;0,VLOOKUP(A21,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Entwicklung von Kalibirerungsobjekten</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>226</v>
+      <c r="D21" s="82" t="s">
+        <v>262</v>
       </c>
       <c r="F21" s="4">
         <v>4</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>282</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -4051,18 +4185,21 @@
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="81">
+      <c r="B22" s="80">
         <v>8</v>
       </c>
-      <c r="C22" s="72" t="str">
+      <c r="C22" s="71" t="str">
         <f>IF(A22&gt;0,VLOOKUP(A22,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Anpassung der Bildverarbeitungs Software</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>227</v>
+      <c r="D22" s="82" t="s">
+        <v>263</v>
       </c>
       <c r="F22" s="4">
         <v>7</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>283</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4073,18 +4210,21 @@
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="81">
+      <c r="B23" s="80">
         <v>8</v>
       </c>
-      <c r="C23" s="72" t="str">
+      <c r="C23" s="71" t="str">
         <f>IF(A23&gt;0,VLOOKUP(A23,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
         <v>Theoretische Darlegung der Bestimmung der Arbeitsbereiche und der Auflösungsgrenzen</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>228</v>
+      <c r="D23" s="82" t="s">
+        <v>264</v>
       </c>
       <c r="F23" s="4">
         <v>5</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>284</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -4117,10 +4257,9 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17">
-      <c r="C27" s="4" t="str">
-        <f>IF(A27&gt;0,VLOOKUP(A27,'Product Backlog'!$A$3:$E$101,3,FALSE),"")</f>
-        <v/>
+    <row r="27" spans="1:17" ht="62">
+      <c r="C27" s="9" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -4569,17 +4708,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="O17:Q17"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="N2:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="O9:Q9"/>
     <mergeCell ref="O13:Q13"/>
     <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O15:Q15"/>
-    <mergeCell ref="O17:Q17"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4607,40 +4746,40 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="19.07421875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="27" style="35" customWidth="1"/>
-    <col min="3" max="3" width="18.765625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="29.69140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="16.07421875" style="30" customWidth="1"/>
-    <col min="6" max="6" width="17.3046875" style="30" customWidth="1"/>
-    <col min="7" max="7" width="15.53515625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="16.69140625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="15.765625" style="30" customWidth="1"/>
-    <col min="10" max="30" width="11.53515625" style="30"/>
+    <col min="1" max="1" width="19.07421875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="27" style="34" customWidth="1"/>
+    <col min="3" max="3" width="18.765625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="29.69140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="16.07421875" style="29" customWidth="1"/>
+    <col min="6" max="6" width="17.3046875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="15.53515625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="16.69140625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="15.765625" style="29" customWidth="1"/>
+    <col min="10" max="30" width="11.53515625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="53.25" customHeight="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="31"/>
+      <c r="A2" s="30"/>
     </row>
     <row r="3" spans="1:30">
-      <c r="A3" s="31"/>
+      <c r="A3" s="30"/>
     </row>
     <row r="4" spans="1:30">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="112" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="119"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
       <c r="E4" s="116">
         <v>1</v>
       </c>
@@ -4648,52 +4787,52 @@
       <c r="G4" s="118"/>
     </row>
     <row r="5" spans="1:30">
-      <c r="A5" s="105"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
+      <c r="A5" s="114"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
       <c r="E5" s="117"/>
       <c r="F5" s="117"/>
       <c r="G5" s="118"/>
     </row>
     <row r="6" spans="1:30">
-      <c r="A6" s="31"/>
+      <c r="A6" s="30"/>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="31"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="50"/>
+      <c r="E7" s="49"/>
       <c r="AA7"/>
       <c r="AB7"/>
       <c r="AC7"/>
       <c r="AD7"/>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="30"/>
       <c r="AA8"/>
       <c r="AB8"/>
       <c r="AC8"/>
       <c r="AD8"/>
     </row>
     <row r="9" spans="1:30" ht="31">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="67">
         <v>1</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="46">
         <v>2</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="43">
         <v>4</v>
       </c>
       <c r="AA9"/>
@@ -4702,18 +4841,18 @@
       <c r="AD9"/>
     </row>
     <row r="10" spans="1:30" ht="31">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="67">
         <f>E4</f>
         <v>1</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="83">
         <f>B10</f>
         <v>1</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="67">
         <f t="shared" ref="D10" si="0">C10</f>
         <v>1</v>
       </c>
@@ -4723,17 +4862,17 @@
       <c r="AD10"/>
     </row>
     <row r="11" spans="1:30" ht="61.5" customHeight="1">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="C11" s="110" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>233</v>
+      <c r="B11" s="81" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>222</v>
       </c>
       <c r="AA11"/>
       <c r="AB11"/>
@@ -4741,16 +4880,16 @@
       <c r="AD11"/>
     </row>
     <row r="12" spans="1:30" ht="31">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="66">
+      <c r="B12" s="65">
         <v>44111</v>
       </c>
-      <c r="C12" s="111">
+      <c r="C12" s="85">
         <v>44111</v>
       </c>
-      <c r="D12" s="66">
+      <c r="D12" s="65">
         <v>44111</v>
       </c>
       <c r="AA12"/>
@@ -4758,32 +4897,32 @@
       <c r="AC12"/>
       <c r="AD12"/>
     </row>
-    <row r="13" spans="1:30" s="30" customFormat="1" ht="46.5">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="1:30" s="29" customFormat="1" ht="46.5">
+      <c r="A13" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="42" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="112" t="s">
-        <v>219</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>219</v>
+      <c r="B13" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:30">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="113" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="D14" s="87" t="s">
+        <v>150</v>
       </c>
       <c r="AA14"/>
       <c r="AB14"/>
@@ -4791,485 +4930,485 @@
       <c r="AD14"/>
     </row>
     <row r="15" spans="1:30" ht="31">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="43"/>
       <c r="AA15"/>
       <c r="AB15"/>
       <c r="AC15"/>
       <c r="AD15"/>
     </row>
     <row r="16" spans="1:30">
-      <c r="A16" s="39"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="44"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="43"/>
       <c r="AA16"/>
       <c r="AB16"/>
       <c r="AC16"/>
       <c r="AD16"/>
     </row>
     <row r="17" spans="1:30" ht="62">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="44"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="43"/>
       <c r="AA17"/>
       <c r="AB17"/>
       <c r="AC17"/>
       <c r="AD17"/>
     </row>
     <row r="18" spans="1:30" ht="62">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="114" t="s">
-        <v>229</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>231</v>
-      </c>
-      <c r="D18" s="121" t="s">
-        <v>248</v>
-      </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="57"/>
+      <c r="B18" s="88" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="90" t="s">
+        <v>235</v>
+      </c>
+      <c r="K18" s="56"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="56"/>
       <c r="AA18"/>
       <c r="AB18"/>
       <c r="AC18"/>
       <c r="AD18"/>
     </row>
     <row r="19" spans="1:30" ht="77.5">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="115" t="s">
-        <v>230</v>
-      </c>
-      <c r="C19" s="76" t="s">
-        <v>232</v>
-      </c>
-      <c r="D19" s="122" t="s">
-        <v>249</v>
-      </c>
-      <c r="K19" s="57"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="57"/>
+      <c r="B19" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="91" t="s">
+        <v>236</v>
+      </c>
+      <c r="K19" s="56"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="56"/>
       <c r="AA19"/>
       <c r="AB19"/>
       <c r="AC19"/>
       <c r="AD19"/>
     </row>
     <row r="20" spans="1:30">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="44"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="43"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
       <c r="AA20"/>
       <c r="AB20"/>
       <c r="AC20"/>
       <c r="AD20"/>
     </row>
     <row r="21" spans="1:30">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="44"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="43"/>
       <c r="AA21"/>
       <c r="AB21"/>
       <c r="AC21"/>
       <c r="AD21"/>
     </row>
     <row r="22" spans="1:30">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="44"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="43"/>
       <c r="AA22"/>
       <c r="AB22"/>
       <c r="AC22"/>
       <c r="AD22"/>
     </row>
     <row r="23" spans="1:30">
-      <c r="A23" s="39"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="44"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="43"/>
       <c r="AA23"/>
       <c r="AB23"/>
       <c r="AC23"/>
       <c r="AD23"/>
     </row>
     <row r="24" spans="1:30">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="44"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="43"/>
       <c r="AA24"/>
       <c r="AB24"/>
       <c r="AC24"/>
       <c r="AD24"/>
     </row>
     <row r="25" spans="1:30">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="44"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="43"/>
       <c r="AA25"/>
       <c r="AB25"/>
       <c r="AC25"/>
       <c r="AD25"/>
     </row>
     <row r="26" spans="1:30">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="44"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="43"/>
       <c r="AA26"/>
       <c r="AB26"/>
       <c r="AC26"/>
       <c r="AD26"/>
     </row>
     <row r="27" spans="1:30">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="44"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="43"/>
       <c r="AA27"/>
       <c r="AB27"/>
       <c r="AC27"/>
       <c r="AD27"/>
     </row>
     <row r="28" spans="1:30">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="44"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="43"/>
       <c r="AA28"/>
       <c r="AB28"/>
       <c r="AC28"/>
       <c r="AD28"/>
     </row>
     <row r="29" spans="1:30">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="44"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="43"/>
       <c r="AA29"/>
       <c r="AB29"/>
       <c r="AC29"/>
       <c r="AD29"/>
     </row>
     <row r="30" spans="1:30">
-      <c r="A30" s="39"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="44"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="43"/>
       <c r="AA30"/>
       <c r="AB30"/>
       <c r="AC30"/>
       <c r="AD30"/>
     </row>
     <row r="31" spans="1:30" ht="46.5">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="44"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="43"/>
       <c r="AA31"/>
       <c r="AB31"/>
       <c r="AC31"/>
       <c r="AD31"/>
     </row>
     <row r="32" spans="1:30">
-      <c r="A32" s="31"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="66" customHeight="1">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="101" t="s">
+      <c r="B33" s="110" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="101"/>
+      <c r="C33" s="110"/>
+      <c r="D33" s="110"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="31"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="27"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="31"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="27"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="31"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="27"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="31"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="101" t="s">
+      <c r="B38" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="101"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
+      <c r="C38" s="110"/>
+      <c r="D38" s="110"/>
+      <c r="E38" s="110"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="110"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="31"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="27"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="31"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="27"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="31"/>
-      <c r="B41" s="28"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="27"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="31"/>
+      <c r="A42" s="30"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="31"/>
+      <c r="A43" s="30"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="31"/>
+      <c r="A44" s="30"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="31"/>
+      <c r="A45" s="30"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="31"/>
+      <c r="A46" s="30"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="31"/>
+      <c r="A47" s="30"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="31"/>
+      <c r="A48" s="30"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="31"/>
+      <c r="A49" s="30"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="31"/>
+      <c r="A50" s="30"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="31"/>
+      <c r="A51" s="30"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="31"/>
+      <c r="A52" s="30"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="31"/>
+      <c r="A53" s="30"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="31"/>
+      <c r="A54" s="30"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="31"/>
+      <c r="A55" s="30"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="31"/>
+      <c r="A56" s="30"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="31"/>
+      <c r="A57" s="30"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="31"/>
+      <c r="A58" s="30"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="31"/>
+      <c r="A59" s="30"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="31"/>
+      <c r="A60" s="30"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="31"/>
+      <c r="A61" s="30"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="31"/>
+      <c r="A62" s="30"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="31"/>
+      <c r="A63" s="30"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="31"/>
+      <c r="A64" s="30"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="31"/>
+      <c r="A65" s="30"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="31"/>
+      <c r="A66" s="30"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="31"/>
+      <c r="A67" s="30"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="31"/>
+      <c r="A68" s="30"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="31"/>
+      <c r="A69" s="30"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="31"/>
+      <c r="A70" s="30"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="31"/>
+      <c r="A71" s="30"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="31"/>
+      <c r="A72" s="30"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="31"/>
+      <c r="A73" s="30"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="31"/>
+      <c r="A74" s="30"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="31"/>
+      <c r="A75" s="30"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="31"/>
+      <c r="A76" s="30"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="31"/>
+      <c r="A77" s="30"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="31"/>
+      <c r="A78" s="30"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="31"/>
+      <c r="A79" s="30"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="31"/>
+      <c r="A80" s="30"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="31"/>
+      <c r="A81" s="30"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="31"/>
+      <c r="A82" s="30"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="31"/>
+      <c r="A83" s="30"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="31"/>
+      <c r="A84" s="30"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="31"/>
+      <c r="A85" s="30"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="31"/>
+      <c r="A86" s="30"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="31"/>
+      <c r="A87" s="30"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="31"/>
+      <c r="A88" s="30"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="31"/>
+      <c r="A89" s="30"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="31"/>
+      <c r="A90" s="30"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="31"/>
+      <c r="A91" s="30"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="31"/>
+      <c r="A92" s="30"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="31"/>
+      <c r="A93" s="30"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="31"/>
+      <c r="A94" s="30"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="31"/>
+      <c r="A95" s="30"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="31"/>
+      <c r="A96" s="30"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="31"/>
+      <c r="A97" s="30"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="31"/>
+      <c r="A98" s="30"/>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="31"/>
+      <c r="A99" s="30"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="31"/>
+      <c r="A100" s="30"/>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="31"/>
+      <c r="A101" s="30"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="31"/>
+      <c r="A102" s="30"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="31"/>
+      <c r="A103" s="30"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="31"/>
+      <c r="A104" s="30"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="31"/>
+      <c r="A105" s="30"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="31"/>
+      <c r="A106" s="30"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="31"/>
+      <c r="A107" s="30"/>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="31"/>
+      <c r="A108" s="30"/>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="31"/>
+      <c r="A109" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5294,8 +5433,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="19.07421875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="61.69140625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="19.07421875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="61.69140625" style="34" customWidth="1"/>
     <col min="3" max="3" width="16.07421875" customWidth="1"/>
     <col min="4" max="4" width="17.3046875" customWidth="1"/>
     <col min="5" max="5" width="15.53515625" customWidth="1"/>
@@ -5303,864 +5442,864 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="53.25" customHeight="1">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="121" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="31"/>
+      <c r="A2" s="30"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="31"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+      <c r="A3" s="30"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="54"/>
+      <c r="A5" s="114"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="31"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="A6" s="30"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="31"/>
-      <c r="B7" s="64" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="31"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="A8" s="30"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:6" ht="31">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="65">
+      <c r="B9" s="64">
         <v>1</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="139.5">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
     <row r="11" spans="1:6" ht="31">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="66">
+      <c r="B11" s="65">
         <v>44095</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-    </row>
-    <row r="12" spans="1:6" s="30" customFormat="1">
-      <c r="A12" s="38" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" s="29" customFormat="1">
+      <c r="A12" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="38"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
     </row>
     <row r="14" spans="1:6" ht="31">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="39"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="1:6" ht="77.5">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
     </row>
     <row r="17" spans="1:5" ht="31">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
     </row>
     <row r="18" spans="1:5" ht="31">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="39"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
     </row>
     <row r="24" spans="1:5" ht="31">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="51"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="31">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
     </row>
     <row r="26" spans="1:5" ht="31">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="39"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="14"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:5" ht="46.5">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
     </row>
     <row r="32" spans="1:5" ht="62">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="B32" s="69" t="s">
+      <c r="B32" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="C32" s="45"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="31"/>
-      <c r="B33" s="71"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="70"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="31"/>
-      <c r="B34" s="71"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="70"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="31"/>
-      <c r="B35" s="28"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="27"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="1:6" ht="170.25" customHeight="1">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="49"/>
-      <c r="B37" s="28"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="27"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="31"/>
-      <c r="B38" s="28"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="27"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="31"/>
-      <c r="B39" s="28"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="27"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="31"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
+      <c r="A40" s="30"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="31"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
+      <c r="A41" s="30"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="31"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
+      <c r="A42" s="30"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="31"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
+      <c r="A43" s="30"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="31"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
+      <c r="A44" s="30"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="31"/>
+      <c r="A45" s="30"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="31"/>
-    </row>
-    <row r="47" spans="1:6" s="33" customFormat="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="35"/>
+      <c r="A46" s="30"/>
+    </row>
+    <row r="47" spans="1:6" s="32" customFormat="1">
+      <c r="A47" s="30"/>
+      <c r="B47" s="34"/>
       <c r="C47"/>
       <c r="D47"/>
       <c r="E47"/>
       <c r="F47"/>
     </row>
-    <row r="48" spans="1:6" s="33" customFormat="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="35"/>
+    <row r="48" spans="1:6" s="32" customFormat="1">
+      <c r="A48" s="30"/>
+      <c r="B48" s="34"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
     </row>
-    <row r="49" spans="1:6" s="33" customFormat="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="35"/>
+    <row r="49" spans="1:6" s="32" customFormat="1">
+      <c r="A49" s="30"/>
+      <c r="B49" s="34"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="1:6" s="33" customFormat="1">
-      <c r="A50" s="31"/>
-      <c r="B50" s="35"/>
+    <row r="50" spans="1:6" s="32" customFormat="1">
+      <c r="A50" s="30"/>
+      <c r="B50" s="34"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
       <c r="F50"/>
     </row>
-    <row r="51" spans="1:6" s="33" customFormat="1">
-      <c r="A51" s="31"/>
-      <c r="B51" s="35"/>
+    <row r="51" spans="1:6" s="32" customFormat="1">
+      <c r="A51" s="30"/>
+      <c r="B51" s="34"/>
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51"/>
     </row>
-    <row r="52" spans="1:6" s="33" customFormat="1">
-      <c r="A52" s="31"/>
-      <c r="B52" s="35"/>
+    <row r="52" spans="1:6" s="32" customFormat="1">
+      <c r="A52" s="30"/>
+      <c r="B52" s="34"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
       <c r="F52"/>
     </row>
-    <row r="53" spans="1:6" s="33" customFormat="1">
-      <c r="A53" s="31"/>
-      <c r="B53" s="35"/>
+    <row r="53" spans="1:6" s="32" customFormat="1">
+      <c r="A53" s="30"/>
+      <c r="B53" s="34"/>
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
       <c r="F53"/>
     </row>
-    <row r="54" spans="1:6" s="33" customFormat="1">
-      <c r="A54" s="31"/>
-      <c r="B54" s="35"/>
+    <row r="54" spans="1:6" s="32" customFormat="1">
+      <c r="A54" s="30"/>
+      <c r="B54" s="34"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54"/>
     </row>
-    <row r="55" spans="1:6" s="33" customFormat="1">
-      <c r="A55" s="31"/>
-      <c r="B55" s="35"/>
+    <row r="55" spans="1:6" s="32" customFormat="1">
+      <c r="A55" s="30"/>
+      <c r="B55" s="34"/>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
       <c r="F55"/>
     </row>
-    <row r="56" spans="1:6" s="33" customFormat="1">
-      <c r="A56" s="31"/>
-      <c r="B56" s="35"/>
+    <row r="56" spans="1:6" s="32" customFormat="1">
+      <c r="A56" s="30"/>
+      <c r="B56" s="34"/>
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56"/>
     </row>
-    <row r="57" spans="1:6" s="33" customFormat="1">
-      <c r="A57" s="31"/>
-      <c r="B57" s="35"/>
+    <row r="57" spans="1:6" s="32" customFormat="1">
+      <c r="A57" s="30"/>
+      <c r="B57" s="34"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57"/>
     </row>
-    <row r="58" spans="1:6" s="33" customFormat="1">
-      <c r="A58" s="31"/>
-      <c r="B58" s="35"/>
+    <row r="58" spans="1:6" s="32" customFormat="1">
+      <c r="A58" s="30"/>
+      <c r="B58" s="34"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
       <c r="F58"/>
     </row>
-    <row r="59" spans="1:6" s="33" customFormat="1">
-      <c r="A59" s="31"/>
-      <c r="B59" s="35"/>
+    <row r="59" spans="1:6" s="32" customFormat="1">
+      <c r="A59" s="30"/>
+      <c r="B59" s="34"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
     </row>
-    <row r="60" spans="1:6" s="33" customFormat="1">
-      <c r="A60" s="31"/>
-      <c r="B60" s="35"/>
+    <row r="60" spans="1:6" s="32" customFormat="1">
+      <c r="A60" s="30"/>
+      <c r="B60" s="34"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
     </row>
-    <row r="61" spans="1:6" s="33" customFormat="1">
-      <c r="A61" s="31"/>
-      <c r="B61" s="35"/>
+    <row r="61" spans="1:6" s="32" customFormat="1">
+      <c r="A61" s="30"/>
+      <c r="B61" s="34"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
     </row>
-    <row r="62" spans="1:6" s="33" customFormat="1">
-      <c r="A62" s="31"/>
-      <c r="B62" s="35"/>
+    <row r="62" spans="1:6" s="32" customFormat="1">
+      <c r="A62" s="30"/>
+      <c r="B62" s="34"/>
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
       <c r="F62"/>
     </row>
-    <row r="63" spans="1:6" s="33" customFormat="1">
-      <c r="A63" s="31"/>
-      <c r="B63" s="35"/>
+    <row r="63" spans="1:6" s="32" customFormat="1">
+      <c r="A63" s="30"/>
+      <c r="B63" s="34"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
       <c r="F63"/>
     </row>
-    <row r="64" spans="1:6" s="33" customFormat="1">
-      <c r="A64" s="31"/>
-      <c r="B64" s="35"/>
+    <row r="64" spans="1:6" s="32" customFormat="1">
+      <c r="A64" s="30"/>
+      <c r="B64" s="34"/>
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
       <c r="F64"/>
     </row>
-    <row r="65" spans="1:6" s="33" customFormat="1">
-      <c r="A65" s="31"/>
-      <c r="B65" s="35"/>
+    <row r="65" spans="1:6" s="32" customFormat="1">
+      <c r="A65" s="30"/>
+      <c r="B65" s="34"/>
       <c r="C65"/>
       <c r="D65"/>
       <c r="E65"/>
       <c r="F65"/>
     </row>
-    <row r="66" spans="1:6" s="33" customFormat="1">
-      <c r="A66" s="31"/>
-      <c r="B66" s="35"/>
+    <row r="66" spans="1:6" s="32" customFormat="1">
+      <c r="A66" s="30"/>
+      <c r="B66" s="34"/>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
       <c r="F66"/>
     </row>
-    <row r="67" spans="1:6" s="33" customFormat="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="35"/>
+    <row r="67" spans="1:6" s="32" customFormat="1">
+      <c r="A67" s="30"/>
+      <c r="B67" s="34"/>
       <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
       <c r="F67"/>
     </row>
-    <row r="68" spans="1:6" s="33" customFormat="1">
-      <c r="A68" s="31"/>
-      <c r="B68" s="35"/>
+    <row r="68" spans="1:6" s="32" customFormat="1">
+      <c r="A68" s="30"/>
+      <c r="B68" s="34"/>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68"/>
       <c r="F68"/>
     </row>
-    <row r="69" spans="1:6" s="33" customFormat="1">
-      <c r="A69" s="31"/>
-      <c r="B69" s="35"/>
+    <row r="69" spans="1:6" s="32" customFormat="1">
+      <c r="A69" s="30"/>
+      <c r="B69" s="34"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
       <c r="F69"/>
     </row>
-    <row r="70" spans="1:6" s="33" customFormat="1">
-      <c r="A70" s="31"/>
-      <c r="B70" s="35"/>
+    <row r="70" spans="1:6" s="32" customFormat="1">
+      <c r="A70" s="30"/>
+      <c r="B70" s="34"/>
       <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
       <c r="F70"/>
     </row>
-    <row r="71" spans="1:6" s="33" customFormat="1">
-      <c r="A71" s="31"/>
-      <c r="B71" s="35"/>
+    <row r="71" spans="1:6" s="32" customFormat="1">
+      <c r="A71" s="30"/>
+      <c r="B71" s="34"/>
       <c r="C71"/>
       <c r="D71"/>
       <c r="E71"/>
       <c r="F71"/>
     </row>
-    <row r="72" spans="1:6" s="33" customFormat="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="35"/>
+    <row r="72" spans="1:6" s="32" customFormat="1">
+      <c r="A72" s="30"/>
+      <c r="B72" s="34"/>
       <c r="C72"/>
       <c r="D72"/>
       <c r="E72"/>
       <c r="F72"/>
     </row>
-    <row r="73" spans="1:6" s="33" customFormat="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="35"/>
+    <row r="73" spans="1:6" s="32" customFormat="1">
+      <c r="A73" s="30"/>
+      <c r="B73" s="34"/>
       <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
       <c r="F73"/>
     </row>
-    <row r="74" spans="1:6" s="33" customFormat="1">
-      <c r="A74" s="31"/>
-      <c r="B74" s="35"/>
+    <row r="74" spans="1:6" s="32" customFormat="1">
+      <c r="A74" s="30"/>
+      <c r="B74" s="34"/>
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
     </row>
-    <row r="75" spans="1:6" s="33" customFormat="1">
-      <c r="A75" s="31"/>
-      <c r="B75" s="35"/>
+    <row r="75" spans="1:6" s="32" customFormat="1">
+      <c r="A75" s="30"/>
+      <c r="B75" s="34"/>
       <c r="C75"/>
       <c r="D75"/>
       <c r="E75"/>
       <c r="F75"/>
     </row>
-    <row r="76" spans="1:6" s="33" customFormat="1">
-      <c r="A76" s="31"/>
-      <c r="B76" s="35"/>
+    <row r="76" spans="1:6" s="32" customFormat="1">
+      <c r="A76" s="30"/>
+      <c r="B76" s="34"/>
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
       <c r="F76"/>
     </row>
-    <row r="77" spans="1:6" s="33" customFormat="1">
-      <c r="A77" s="31"/>
-      <c r="B77" s="35"/>
+    <row r="77" spans="1:6" s="32" customFormat="1">
+      <c r="A77" s="30"/>
+      <c r="B77" s="34"/>
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
       <c r="F77"/>
     </row>
-    <row r="78" spans="1:6" s="33" customFormat="1">
-      <c r="A78" s="31"/>
-      <c r="B78" s="35"/>
+    <row r="78" spans="1:6" s="32" customFormat="1">
+      <c r="A78" s="30"/>
+      <c r="B78" s="34"/>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78"/>
     </row>
-    <row r="79" spans="1:6" s="33" customFormat="1">
-      <c r="A79" s="31"/>
-      <c r="B79" s="35"/>
+    <row r="79" spans="1:6" s="32" customFormat="1">
+      <c r="A79" s="30"/>
+      <c r="B79" s="34"/>
       <c r="C79"/>
       <c r="D79"/>
       <c r="E79"/>
       <c r="F79"/>
     </row>
-    <row r="80" spans="1:6" s="33" customFormat="1">
-      <c r="A80" s="31"/>
-      <c r="B80" s="35"/>
+    <row r="80" spans="1:6" s="32" customFormat="1">
+      <c r="A80" s="30"/>
+      <c r="B80" s="34"/>
       <c r="C80"/>
       <c r="D80"/>
       <c r="E80"/>
       <c r="F80"/>
     </row>
-    <row r="81" spans="1:6" s="33" customFormat="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="35"/>
+    <row r="81" spans="1:6" s="32" customFormat="1">
+      <c r="A81" s="30"/>
+      <c r="B81" s="34"/>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
       <c r="F81"/>
     </row>
-    <row r="82" spans="1:6" s="33" customFormat="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="35"/>
+    <row r="82" spans="1:6" s="32" customFormat="1">
+      <c r="A82" s="30"/>
+      <c r="B82" s="34"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
       <c r="F82"/>
     </row>
-    <row r="83" spans="1:6" s="33" customFormat="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="35"/>
+    <row r="83" spans="1:6" s="32" customFormat="1">
+      <c r="A83" s="30"/>
+      <c r="B83" s="34"/>
       <c r="C83"/>
       <c r="D83"/>
       <c r="E83"/>
       <c r="F83"/>
     </row>
-    <row r="84" spans="1:6" s="33" customFormat="1">
-      <c r="A84" s="31"/>
-      <c r="B84" s="35"/>
+    <row r="84" spans="1:6" s="32" customFormat="1">
+      <c r="A84" s="30"/>
+      <c r="B84" s="34"/>
       <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
       <c r="F84"/>
     </row>
-    <row r="85" spans="1:6" s="33" customFormat="1">
-      <c r="A85" s="31"/>
-      <c r="B85" s="35"/>
+    <row r="85" spans="1:6" s="32" customFormat="1">
+      <c r="A85" s="30"/>
+      <c r="B85" s="34"/>
       <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85"/>
     </row>
-    <row r="86" spans="1:6" s="33" customFormat="1">
-      <c r="A86" s="31"/>
-      <c r="B86" s="35"/>
+    <row r="86" spans="1:6" s="32" customFormat="1">
+      <c r="A86" s="30"/>
+      <c r="B86" s="34"/>
       <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86"/>
     </row>
-    <row r="87" spans="1:6" s="33" customFormat="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="35"/>
+    <row r="87" spans="1:6" s="32" customFormat="1">
+      <c r="A87" s="30"/>
+      <c r="B87" s="34"/>
       <c r="C87"/>
       <c r="D87"/>
       <c r="E87"/>
       <c r="F87"/>
     </row>
-    <row r="88" spans="1:6" s="33" customFormat="1">
-      <c r="A88" s="31"/>
-      <c r="B88" s="35"/>
+    <row r="88" spans="1:6" s="32" customFormat="1">
+      <c r="A88" s="30"/>
+      <c r="B88" s="34"/>
       <c r="C88"/>
       <c r="D88"/>
       <c r="E88"/>
       <c r="F88"/>
     </row>
-    <row r="89" spans="1:6" s="33" customFormat="1">
-      <c r="A89" s="31"/>
-      <c r="B89" s="35"/>
+    <row r="89" spans="1:6" s="32" customFormat="1">
+      <c r="A89" s="30"/>
+      <c r="B89" s="34"/>
       <c r="C89"/>
       <c r="D89"/>
       <c r="E89"/>
       <c r="F89"/>
     </row>
-    <row r="90" spans="1:6" s="33" customFormat="1">
-      <c r="A90" s="31"/>
-      <c r="B90" s="35"/>
+    <row r="90" spans="1:6" s="32" customFormat="1">
+      <c r="A90" s="30"/>
+      <c r="B90" s="34"/>
       <c r="C90"/>
       <c r="D90"/>
       <c r="E90"/>
       <c r="F90"/>
     </row>
-    <row r="91" spans="1:6" s="33" customFormat="1">
-      <c r="A91" s="31"/>
-      <c r="B91" s="35"/>
+    <row r="91" spans="1:6" s="32" customFormat="1">
+      <c r="A91" s="30"/>
+      <c r="B91" s="34"/>
       <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
       <c r="F91"/>
     </row>
-    <row r="92" spans="1:6" s="33" customFormat="1">
-      <c r="A92" s="31"/>
-      <c r="B92" s="35"/>
+    <row r="92" spans="1:6" s="32" customFormat="1">
+      <c r="A92" s="30"/>
+      <c r="B92" s="34"/>
       <c r="C92"/>
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92"/>
     </row>
-    <row r="93" spans="1:6" s="33" customFormat="1">
-      <c r="A93" s="31"/>
-      <c r="B93" s="35"/>
+    <row r="93" spans="1:6" s="32" customFormat="1">
+      <c r="A93" s="30"/>
+      <c r="B93" s="34"/>
       <c r="C93"/>
       <c r="D93"/>
       <c r="E93"/>
       <c r="F93"/>
     </row>
-    <row r="94" spans="1:6" s="33" customFormat="1">
-      <c r="A94" s="31"/>
-      <c r="B94" s="35"/>
+    <row r="94" spans="1:6" s="32" customFormat="1">
+      <c r="A94" s="30"/>
+      <c r="B94" s="34"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
       <c r="F94"/>
     </row>
-    <row r="95" spans="1:6" s="33" customFormat="1">
-      <c r="A95" s="31"/>
-      <c r="B95" s="35"/>
+    <row r="95" spans="1:6" s="32" customFormat="1">
+      <c r="A95" s="30"/>
+      <c r="B95" s="34"/>
       <c r="C95"/>
       <c r="D95"/>
       <c r="E95"/>
       <c r="F95"/>
     </row>
-    <row r="96" spans="1:6" s="33" customFormat="1">
-      <c r="A96" s="31"/>
-      <c r="B96" s="35"/>
+    <row r="96" spans="1:6" s="32" customFormat="1">
+      <c r="A96" s="30"/>
+      <c r="B96" s="34"/>
       <c r="C96"/>
       <c r="D96"/>
       <c r="E96"/>
       <c r="F96"/>
     </row>
-    <row r="97" spans="1:6" s="33" customFormat="1">
-      <c r="A97" s="31"/>
-      <c r="B97" s="35"/>
+    <row r="97" spans="1:6" s="32" customFormat="1">
+      <c r="A97" s="30"/>
+      <c r="B97" s="34"/>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
       <c r="F97"/>
     </row>
-    <row r="98" spans="1:6" s="33" customFormat="1">
-      <c r="A98" s="31"/>
-      <c r="B98" s="35"/>
+    <row r="98" spans="1:6" s="32" customFormat="1">
+      <c r="A98" s="30"/>
+      <c r="B98" s="34"/>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
       <c r="F98"/>
     </row>
-    <row r="99" spans="1:6" s="33" customFormat="1">
-      <c r="A99" s="31"/>
-      <c r="B99" s="35"/>
+    <row r="99" spans="1:6" s="32" customFormat="1">
+      <c r="A99" s="30"/>
+      <c r="B99" s="34"/>
       <c r="C99"/>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99"/>
     </row>
-    <row r="100" spans="1:6" s="33" customFormat="1">
-      <c r="A100" s="31"/>
-      <c r="B100" s="35"/>
+    <row r="100" spans="1:6" s="32" customFormat="1">
+      <c r="A100" s="30"/>
+      <c r="B100" s="34"/>
       <c r="C100"/>
       <c r="D100"/>
       <c r="E100"/>
       <c r="F100"/>
     </row>
-    <row r="101" spans="1:6" s="33" customFormat="1">
-      <c r="A101" s="31"/>
-      <c r="B101" s="35"/>
+    <row r="101" spans="1:6" s="32" customFormat="1">
+      <c r="A101" s="30"/>
+      <c r="B101" s="34"/>
       <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
     </row>
-    <row r="102" spans="1:6" s="33" customFormat="1">
-      <c r="A102" s="31"/>
-      <c r="B102" s="35"/>
+    <row r="102" spans="1:6" s="32" customFormat="1">
+      <c r="A102" s="30"/>
+      <c r="B102" s="34"/>
       <c r="C102"/>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
     </row>
-    <row r="103" spans="1:6" s="33" customFormat="1">
-      <c r="A103" s="31"/>
-      <c r="B103" s="35"/>
+    <row r="103" spans="1:6" s="32" customFormat="1">
+      <c r="A103" s="30"/>
+      <c r="B103" s="34"/>
       <c r="C103"/>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
     </row>
-    <row r="104" spans="1:6" s="33" customFormat="1">
-      <c r="A104" s="31"/>
-      <c r="B104" s="35"/>
+    <row r="104" spans="1:6" s="32" customFormat="1">
+      <c r="A104" s="30"/>
+      <c r="B104" s="34"/>
       <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
     </row>
-    <row r="105" spans="1:6" s="33" customFormat="1">
-      <c r="A105" s="31"/>
-      <c r="B105" s="35"/>
+    <row r="105" spans="1:6" s="32" customFormat="1">
+      <c r="A105" s="30"/>
+      <c r="B105" s="34"/>
       <c r="C105"/>
       <c r="D105"/>
       <c r="E105"/>
       <c r="F105"/>
     </row>
-    <row r="106" spans="1:6" s="33" customFormat="1">
-      <c r="A106" s="31"/>
-      <c r="B106" s="35"/>
+    <row r="106" spans="1:6" s="32" customFormat="1">
+      <c r="A106" s="30"/>
+      <c r="B106" s="34"/>
       <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
       <c r="F106"/>
     </row>
-    <row r="107" spans="1:6" s="33" customFormat="1">
-      <c r="A107" s="31"/>
-      <c r="B107" s="35"/>
+    <row r="107" spans="1:6" s="32" customFormat="1">
+      <c r="A107" s="30"/>
+      <c r="B107" s="34"/>
       <c r="C107"/>
       <c r="D107"/>
       <c r="E107"/>
       <c r="F107"/>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="31"/>
+      <c r="A108" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>